<commit_message>
Updated the burn deck
</commit_message>
<xml_diff>
--- a/monoRedBruno.xlsx
+++ b/monoRedBruno.xlsx
@@ -95,15 +95,6 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -464,19 +455,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="23.41" customWidth="1" style="3" min="1" max="1"/>
+    <col width="38.98" customWidth="1" style="3" min="1" max="1"/>
     <col width="25.63" customWidth="1" style="3" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="4">
+    <row r="1" ht="12.75" customHeight="1" s="4">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
@@ -503,15 +494,15 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="4">
+    <row r="2" ht="12.75" customHeight="1" s="4">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Bomat Courier</t>
+          <t>Bonecrusher Giant: Stomp</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>Kaladesh</t>
+          <t>Throne of Eldraine</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -520,7 +511,7 @@
         </is>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.33</v>
+        <v>0.71</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>4</v>
@@ -530,15 +521,15 @@
         <v/>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="4">
+    <row r="3" ht="12.75" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Bonecrusher Giant: Stomp</t>
+          <t>Electrostatic Infantry</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Throne of Eldraine</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -547,17 +538,17 @@
         </is>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.59</v>
+        <v>0.18</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5">
         <f>D3*E3</f>
         <v/>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="4">
+    <row r="4" ht="12.75" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Ghitu Lavarunner</t>
@@ -574,7 +565,7 @@
         </is>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>4</v>
@@ -584,15 +575,15 @@
         <v/>
       </c>
     </row>
-    <row r="5" ht="12.8" customHeight="1" s="4">
+    <row r="5" ht="12.75" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Light Up the Stage</t>
+          <t>Kumano Faces Kakkazan: Etching of Kumano</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Ravnica Allegiance</t>
+          <t>Kamigawa: Neon Dynasty</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -601,25 +592,25 @@
         </is>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5" s="5">
         <f>D5*E5</f>
         <v/>
       </c>
     </row>
-    <row r="6" ht="12.8" customHeight="1" s="4">
+    <row r="6" ht="12.75" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Lightning Strike</t>
+          <t>Light Up the Stage</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Core 2019</t>
+          <t>Ravnica Allegiance</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -628,7 +619,7 @@
         </is>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.08</v>
+        <v>0.23</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>4</v>
@@ -638,15 +629,15 @@
         <v/>
       </c>
     </row>
-    <row r="7" ht="12.8" customHeight="1" s="4">
+    <row r="7" ht="12.75" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Monastery Swiftspear</t>
+          <t>Lightning Strike</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>Core 2019</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -655,25 +646,25 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.59</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="5">
         <f>D7*E7</f>
         <v/>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="4">
+    <row r="8" ht="12.75" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Ramunap Ruins</t>
+          <t>Lightning Strike</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Hour of Devastation</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -682,25 +673,25 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.51</v>
+        <v>0.29</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5">
         <f>D8*E8</f>
         <v/>
       </c>
     </row>
-    <row r="9" ht="12.8" customHeight="1" s="4">
+    <row r="9" ht="12.75" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Soul-Scar Mage</t>
+          <t>Monastery Swiftspear</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Amonkhet</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -709,7 +700,7 @@
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>1.93</v>
+        <v>0.59</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>4</v>
@@ -719,15 +710,15 @@
         <v/>
       </c>
     </row>
-    <row r="10" ht="12.8" customHeight="1" s="4">
+    <row r="10" ht="12.75" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Viashino Pyromancer</t>
+          <t>Phoenix Chick</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Core 2019</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -736,25 +727,25 @@
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0.09</v>
+        <v>0.25</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="5">
         <f>D10*E10</f>
         <v/>
       </c>
     </row>
-    <row r="11" ht="12.8" customHeight="1" s="4">
+    <row r="11" ht="12.75" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Wild Slash</t>
+          <t>Ramunap Ruins</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Magic the Gathering Products</t>
+          <t>Hour of Devastation</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -763,7 +754,7 @@
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0.25</v>
+        <v>0.62</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>4</v>
@@ -773,15 +764,15 @@
         <v/>
       </c>
     </row>
-    <row r="12" ht="12.8" customHeight="1" s="4">
+    <row r="12" ht="12.75" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Wizard's Lightning</t>
+          <t>Soul-Scar Mage</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Dominaria</t>
+          <t>Amonkhet</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -790,7 +781,7 @@
         </is>
       </c>
       <c r="D12" s="5" t="n">
-        <v>0.18</v>
+        <v>1.88</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>4</v>
@@ -799,20 +790,16 @@
         <f>D12*E12</f>
         <v/>
       </c>
-      <c r="G12" s="5">
-        <f>SUM(F2:F12)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" ht="12.8" customHeight="1" s="4">
+    </row>
+    <row r="13" ht="12.75" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Chandra, Torch of Defiance</t>
+          <t>Viashino Pyromancer</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Magic the Gathering Products</t>
+          <t>Core 2019</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -821,25 +808,25 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>7.07</v>
+        <v>0.1</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="5">
         <f>D13*E13</f>
         <v/>
       </c>
     </row>
-    <row r="14" ht="12.8" customHeight="1" s="4">
+    <row r="14" ht="12.75" customHeight="1" s="4">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Goblin Chainwhirler</t>
+          <t>Wild Slash</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Dominaria</t>
+          <t>Magic the Gathering Products</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -848,25 +835,25 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.58</v>
+        <v>0.23</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="5">
         <f>D14*E14</f>
         <v/>
       </c>
     </row>
-    <row r="15" ht="12.8" customHeight="1" s="4">
+    <row r="15" ht="12.75" customHeight="1" s="4">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Searing Blood</t>
+          <t>Wizard's Lightning</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Magic the Gathering Products</t>
+          <t>Dominaria</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -875,7 +862,7 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.26</v>
+        <v>0.18</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>4</v>
@@ -884,16 +871,17 @@
         <f>D15*E15</f>
         <v/>
       </c>
-    </row>
-    <row r="16" ht="12.8" customHeight="1" s="4">
+      <c r="G15" s="5" t="n"/>
+    </row>
+    <row r="16" ht="12.75" customHeight="1" s="4">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Roiling Vortex</t>
+          <t>Young Pyromancer</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Zendikar Rising</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -902,25 +890,26 @@
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0.48</v>
+        <v>0.28</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5">
         <f>D16*E16</f>
         <v/>
       </c>
-    </row>
-    <row r="17" ht="12.8" customHeight="1" s="4">
+      <c r="G16" s="5" t="n"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1" s="4">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Magma Spray</t>
+          <t>Young Pyromancer</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Amonkhet</t>
+          <t>Magic 2014</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -929,23 +918,162 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.02</v>
+        <v>0.24</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" s="5">
         <f>D17*E17</f>
         <v/>
       </c>
       <c r="G17" s="5">
-        <f>SUM(F13:F17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" ht="12.8" customHeight="1" s="4">
+        <f>SUM(F2:F17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1" s="4">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Chandra, Torch of Defiance</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Magic the Gathering Products</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>7.18</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="F18" s="5">
-        <f>SUM(F2:F17)</f>
+        <f>D18*E18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1" s="4">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Goblin Chainwhirler</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Dominaria</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" s="5">
+        <f>D19*E19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="4">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Searing Blood</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Magic the Gathering Products</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5">
+        <f>D20*E20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="4">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>Roiling Vortex</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Zendikar Rising</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="5">
+        <f>D21*E21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" ht="12.75" customHeight="1" s="4">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>Magma Spray</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Amonkhet</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
+        <f>D22*E22</f>
+        <v/>
+      </c>
+      <c r="G22" s="5">
+        <f>SUM(F18:F22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" ht="12.75" customHeight="1" s="4">
+      <c r="F23" s="5">
+        <f>SUM(F2:F22)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Upgraded Bruno, now it's even cheaper
</commit_message>
<xml_diff>
--- a/monoRedBruno.xlsx
+++ b/monoRedBruno.xlsx
@@ -455,10 +455,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -511,10 +511,10 @@
         </is>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="5">
         <f>D2*E2</f>
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>4</v>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>1</v>
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.28</v>
+        <v>0.24</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>4</v>
@@ -646,10 +646,10 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" s="5">
         <f>D7*E7</f>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>1</v>
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>4</v>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>4</v>
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="D12" s="5" t="n">
-        <v>1.99</v>
+        <v>1.94</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>4</v>
@@ -794,12 +794,12 @@
     <row r="13" ht="12.75" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Viashino Pyromancer</t>
+          <t>Sticky Fingers</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Core 2019</t>
+          <t>Streets of New Capenna</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>2</v>
@@ -821,12 +821,12 @@
     <row r="14" ht="12.75" customHeight="1" s="4">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Wild Slash</t>
+          <t>Titan's Strength</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Magic the Gathering Products</t>
+          <t>Magic Origins</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -835,10 +835,10 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.21</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" s="5">
         <f>D14*E14</f>
@@ -848,12 +848,12 @@
     <row r="15" ht="12.75" customHeight="1" s="4">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Wizard's Lightning</t>
+          <t>Titan's Strength</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Dominaria</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -862,26 +862,25 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F15" s="5">
         <f>D15*E15</f>
         <v/>
       </c>
-      <c r="G15" s="5" t="n"/>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="4">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Young Pyromancer</t>
+          <t>Viashino Pyromancer</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Core 2019</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -890,26 +889,25 @@
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="5">
         <f>D16*E16</f>
         <v/>
       </c>
-      <c r="G16" s="5" t="n"/>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="4">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Young Pyromancer</t>
+          <t>Wild Slash</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Magic 2014</t>
+          <t>Magic the Gathering Products</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -918,29 +916,25 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.48</v>
+        <v>0.22</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F17" s="5">
         <f>D17*E17</f>
         <v/>
       </c>
-      <c r="G17" s="5">
-        <f>SUM(F2:F17)</f>
-        <v/>
-      </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" s="4">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Chandra, Torch of Defiance</t>
+          <t>Wizard's Lightning</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Magic the Gathering Products</t>
+          <t>Dominaria</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -949,25 +943,29 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>3.04</v>
+        <v>0.16</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" s="5">
         <f>D18*E18</f>
         <v/>
       </c>
+      <c r="G18" s="5">
+        <f>SUM(F2:F18)</f>
+        <v/>
+      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1" s="4">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Goblin Chainwhirler</t>
+          <t>Chandra, Torch of Defiance</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Dominaria</t>
+          <t>Magic the Gathering Products</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -976,10 +974,10 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.52</v>
+        <v>3.03</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5">
         <f>D19*E19</f>
@@ -989,12 +987,12 @@
     <row r="20" ht="12.75" customHeight="1" s="4">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Searing Blood</t>
+          <t>Goblin Chainwhirler</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Magic the Gathering Products</t>
+          <t>Dominaria</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1003,10 +1001,10 @@
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0.31</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" s="5">
         <f>D20*E20</f>
@@ -1016,12 +1014,12 @@
     <row r="21" ht="12.75" customHeight="1" s="4">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Roiling Vortex</t>
+          <t>Searing Blood</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Zendikar Rising</t>
+          <t>Magic the Gathering Products</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1030,7 +1028,7 @@
         </is>
       </c>
       <c r="D21" s="5" t="n">
-        <v>0.58</v>
+        <v>0.27</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>4</v>
@@ -1043,12 +1041,12 @@
     <row r="22" ht="12.75" customHeight="1" s="4">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Magma Spray</t>
+          <t>Roiling Vortex</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Amonkhet</t>
+          <t>Zendikar Rising</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1057,27 +1055,53 @@
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>0.09</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F22" s="5">
         <f>D22*E22</f>
         <v/>
       </c>
-      <c r="G22" s="5">
-        <f>SUM(F18:F22)</f>
-        <v/>
-      </c>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="4">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>Magma Spray</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Amonkhet</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="F23" s="5">
-        <f>SUM(F2:F22)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1048576" ht="12.8" customHeight="1" s="4"/>
+        <f>D23*E23</f>
+        <v/>
+      </c>
+      <c r="G23" s="5">
+        <f>SUM(F19:F23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" ht="12.75" customHeight="1" s="4">
+      <c r="F24" s="5">
+        <f>SUM(F2:F23)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>